<commit_message>
add tailwind, remake ui, edit redme
</commit_message>
<xml_diff>
--- a/sprint agile.xlsx
+++ b/sprint agile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adekgita\Documents\Kuliah\Semester 7\Praktikum\Modul 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03661B3B-CC6A-42A9-9BF0-0C9B43DC55EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABA3BCA-A3FA-4D01-8148-853841A299F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{5B4B256B-9975-4767-9612-A8B9F079D775}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5B4B256B-9975-4767-9612-A8B9F079D775}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>no</t>
   </si>
@@ -60,9 +60,6 @@
     <t>setup environtment</t>
   </si>
   <si>
-    <t>setup environtment backend(routing dll)</t>
-  </si>
-  <si>
     <t>web interface</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>2 jam</t>
   </si>
   <si>
-    <t>ON PROGRESS</t>
-  </si>
-  <si>
     <t>20 menit</t>
   </si>
   <si>
@@ -106,6 +100,9 @@
   </si>
   <si>
     <t>5 menit</t>
+  </si>
+  <si>
+    <t>setup backend(routing dll)</t>
   </si>
 </sst>
 </file>
@@ -233,9 +230,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -244,7 +240,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39987FDB-C63F-4609-BEB8-1E03E077207F}">
   <dimension ref="B2:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,19 +570,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H2" t="s">
@@ -595,139 +590,139 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
         <v>8</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="8">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="8">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="8">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>